<commit_message>
balance between class and gender
</commit_message>
<xml_diff>
--- a/split_them.xlsx
+++ b/split_them.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ubuntu\python\classMaker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ubuntu\python\classMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2FDC02-4FD0-4BDD-8682-B2AF8C78E39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1289DC-5B2D-4715-B605-3F6EB2EC9C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="1725" windowWidth="14130" windowHeight="12255" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,30 +20,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>예시101</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>예시102</t>
-  </si>
-  <si>
-    <t>예시103</t>
-  </si>
-  <si>
-    <t>예시105</t>
-  </si>
-  <si>
-    <t>예시201</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>예시202</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>예시401</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시111</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시112</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시113</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시211</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시213</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시314</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시510</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시415</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>예시619</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -367,41 +382,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>